<commit_message>
Planning updated with dates
</commit_message>
<xml_diff>
--- a/Iteration Planning.xlsx
+++ b/Iteration Planning.xlsx
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>Setup SVN</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Check in existing diagrams:
 Use Cases, Domain Model,
@@ -69,17 +63,41 @@
     <t>Write code in skeleton classes</t>
   </si>
   <si>
-    <t>Create skeleton classes</t>
-  </si>
-  <si>
     <t>Study GRASP patterns if not yet done</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Setup SVN/Github</t>
+  </si>
+  <si>
+    <t>Create skeleton classes/methods</t>
+  </si>
+  <si>
+    <t>Identify/Create Controller</t>
+  </si>
+  <si>
+    <t>Revise</t>
+  </si>
+  <si>
+    <t>Parking Garage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,13 +105,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,11 +155,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,106 +469,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2">
+        <v>41914</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" t="s">
+      <c r="G4" s="2">
+        <v>41914</v>
+      </c>
+      <c r="I4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="C5" s="2">
+        <v>41915</v>
+      </c>
+      <c r="D5" s="2">
+        <v>41915</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>41916</v>
+      </c>
+      <c r="D6" s="2">
+        <v>41916</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>41917</v>
+      </c>
+      <c r="D7" s="2">
+        <v>41917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>41918</v>
+      </c>
+      <c r="D8" s="2">
+        <v>41918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>41916</v>
+      </c>
+      <c r="D9" s="2">
+        <v>41919</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2">
+        <v>41933</v>
+      </c>
+      <c r="D10" s="2">
+        <v>41934</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2">
+        <v>41935</v>
+      </c>
+      <c r="D11" s="2">
+        <v>41937</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2">
+        <v>41916</v>
+      </c>
+      <c r="D12" s="2">
+        <v>41916</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2">
+        <v>41921</v>
+      </c>
+      <c r="D13" s="2">
+        <v>41921</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2">
+        <v>41920</v>
+      </c>
+      <c r="D14" s="2">
+        <v>41921</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2">
+        <v>41922</v>
+      </c>
+      <c r="D15" s="2">
+        <v>41922</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="C16" s="2">
+        <v>41923</v>
+      </c>
+      <c r="D16" s="2">
+        <v>41927</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
+      <c r="C17" s="2">
+        <v>41928</v>
+      </c>
+      <c r="D17" s="2">
+        <v>74804</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2">
+        <v>41938</v>
+      </c>
+      <c r="D18" s="2">
+        <v>41941</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>